<commit_message>
updates datasets, still some site messyness on early data but otherwise complete
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_survey_charachteristics_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_survey_charachteristics_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erincain/Documents/Git/edi-feather-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF0F9F2-3FBC-0C41-8560-DCEFEA37D9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C353896B-7D9B-F24F-BFC4-C15C2D437CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -106,19 +106,10 @@
     <t xml:space="preserve">temperature          </t>
   </si>
   <si>
-    <t xml:space="preserve">start_time          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">end_time             </t>
-  </si>
-  <si>
     <t xml:space="preserve">section_name        </t>
   </si>
   <si>
     <t xml:space="preserve">units_covered        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">unit                 </t>
   </si>
   <si>
     <t>interval</t>
@@ -136,22 +127,10 @@
     <t>Turbidity measured at survey</t>
   </si>
   <si>
-    <t>Time when snorkel survey started</t>
-  </si>
-  <si>
     <t xml:space="preserve">weather      </t>
   </si>
   <si>
-    <t xml:space="preserve">hydrology    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">visibility </t>
-  </si>
-  <si>
     <t>dateTime</t>
-  </si>
-  <si>
-    <t>meter</t>
   </si>
   <si>
     <t>Identification number of survey</t>
@@ -169,43 +148,27 @@
     <t>YYYY-MM-DD</t>
   </si>
   <si>
-    <t>hh:mm:ss</t>
-  </si>
-  <si>
     <t>NTU</t>
   </si>
   <si>
     <t>Flow in cubic feet per seccond (cfs)</t>
   </si>
   <si>
-    <t>Time when snorkel survey ended</t>
-  </si>
-  <si>
-    <t>Location were snorkel data was collected.</t>
-  </si>
-  <si>
     <t>Units surveyed on a given snorkel suvey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit associated with specific reccord observed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distance under current conditions of how far you can see/identify a fish. Recorded in meters. </t>
   </si>
   <si>
     <t>Weather conditions when data was collected. Weather conditions include: clear, sunny, clear and windy, cloudy, partly cloudy, precipitation, hazy, windy, clear and hot, overcast</t>
   </si>
   <si>
-    <t>Hydological features at study site. Features include: riffle, glide, glide edgewater, riffle edgewater, backwater, pool)</t>
+    <t>Section name describing location were snorkel data was collected.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
@@ -267,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -298,16 +261,10 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="21" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -537,17 +494,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z983"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15:XFD15"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="42" style="21" customWidth="1"/>
+    <col min="2" max="2" width="42" style="19" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
@@ -620,13 +577,13 @@
         <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>14</v>
@@ -658,29 +615,29 @@
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="2"/>
       <c r="J3" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="K3" s="6"/>
-      <c r="L3" s="16">
+      <c r="L3" s="15">
         <v>36259</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M3" s="15">
         <v>44099</v>
       </c>
       <c r="N3" s="1"/>
@@ -702,13 +659,13 @@
         <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>16</v>
@@ -717,7 +674,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>17</v>
@@ -747,16 +704,16 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -788,13 +745,13 @@
         <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
@@ -803,7 +760,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>17</v>
@@ -836,31 +793,25 @@
         <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="J7" s="5"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="17">
-        <v>4.8611111111111112E-2</v>
-      </c>
-      <c r="M7" s="17">
-        <v>0.98611111111111116</v>
-      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="3"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -879,32 +830,26 @@
       <c r="A8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>50</v>
+      <c r="B8" s="17" t="s">
+        <v>42</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="J8" s="5"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="17">
-        <v>5.0694444444444445E-2</v>
-      </c>
-      <c r="M8" s="17">
-        <v>0.66111111111111109</v>
-      </c>
+      <c r="L8" s="7"/>
+      <c r="M8" s="3"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -921,28 +866,38 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>51</v>
+      <c r="G9" s="3" t="s">
+        <v>30</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
+      <c r="H9" s="3" t="s">
+        <v>17</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="3"/>
+      <c r="L9" s="14">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3">
+        <v>21.67</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -957,194 +912,67 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-    </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="M12" s="14">
-        <v>9</v>
-      </c>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
+      <c r="A12" s="4"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="2"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
       <c r="J13" s="5"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="15">
-        <v>0</v>
-      </c>
-      <c r="M13" s="3">
-        <v>21.67</v>
-      </c>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-    </row>
-    <row r="14" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1167,32 +995,79 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K15" s="2"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+    </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
+      <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
@@ -1200,27 +1075,27 @@
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
@@ -1251,6 +1126,16 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="3"/>
       <c r="K20" s="2"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
@@ -1269,7 +1154,6 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
@@ -1325,7 +1209,6 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
@@ -1409,6 +1292,7 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="2"/>
@@ -1464,6 +1348,7 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
@@ -2303,7 +2188,7 @@
       <c r="Z57" s="1"/>
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="4"/>
+      <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="2"/>
@@ -2331,7 +2216,7 @@
       <c r="Z58" s="1"/>
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="4"/>
+      <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="2"/>
@@ -2359,7 +2244,7 @@
       <c r="Z59" s="1"/>
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="4"/>
+      <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="2"/>
@@ -2387,7 +2272,7 @@
       <c r="Z60" s="1"/>
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="4"/>
+      <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="2"/>
@@ -2415,7 +2300,7 @@
       <c r="Z61" s="1"/>
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="4"/>
+      <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="2"/>
@@ -28230,158 +28115,18 @@
       <c r="Y983" s="1"/>
       <c r="Z983" s="1"/>
     </row>
-    <row r="984" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A984" s="1"/>
-      <c r="B984" s="1"/>
-      <c r="C984" s="1"/>
-      <c r="D984" s="2"/>
-      <c r="E984" s="1"/>
-      <c r="F984" s="3"/>
-      <c r="G984" s="3"/>
-      <c r="H984" s="3"/>
-      <c r="I984" s="2"/>
-      <c r="J984" s="3"/>
-      <c r="K984" s="2"/>
-      <c r="L984" s="3"/>
-      <c r="M984" s="3"/>
-      <c r="N984" s="1"/>
-      <c r="O984" s="1"/>
-      <c r="P984" s="1"/>
-      <c r="Q984" s="1"/>
-      <c r="R984" s="1"/>
-      <c r="S984" s="1"/>
-      <c r="T984" s="1"/>
-      <c r="U984" s="1"/>
-      <c r="V984" s="1"/>
-      <c r="W984" s="1"/>
-      <c r="X984" s="1"/>
-      <c r="Y984" s="1"/>
-      <c r="Z984" s="1"/>
-    </row>
-    <row r="985" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A985" s="1"/>
-      <c r="B985" s="1"/>
-      <c r="C985" s="1"/>
-      <c r="D985" s="2"/>
-      <c r="E985" s="1"/>
-      <c r="F985" s="3"/>
-      <c r="G985" s="3"/>
-      <c r="H985" s="3"/>
-      <c r="I985" s="2"/>
-      <c r="J985" s="3"/>
-      <c r="K985" s="2"/>
-      <c r="L985" s="3"/>
-      <c r="M985" s="3"/>
-      <c r="N985" s="1"/>
-      <c r="O985" s="1"/>
-      <c r="P985" s="1"/>
-      <c r="Q985" s="1"/>
-      <c r="R985" s="1"/>
-      <c r="S985" s="1"/>
-      <c r="T985" s="1"/>
-      <c r="U985" s="1"/>
-      <c r="V985" s="1"/>
-      <c r="W985" s="1"/>
-      <c r="X985" s="1"/>
-      <c r="Y985" s="1"/>
-      <c r="Z985" s="1"/>
-    </row>
-    <row r="986" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A986" s="1"/>
-      <c r="B986" s="1"/>
-      <c r="C986" s="1"/>
-      <c r="D986" s="2"/>
-      <c r="E986" s="1"/>
-      <c r="F986" s="3"/>
-      <c r="G986" s="3"/>
-      <c r="H986" s="3"/>
-      <c r="I986" s="2"/>
-      <c r="J986" s="3"/>
-      <c r="K986" s="2"/>
-      <c r="L986" s="3"/>
-      <c r="M986" s="3"/>
-      <c r="N986" s="1"/>
-      <c r="O986" s="1"/>
-      <c r="P986" s="1"/>
-      <c r="Q986" s="1"/>
-      <c r="R986" s="1"/>
-      <c r="S986" s="1"/>
-      <c r="T986" s="1"/>
-      <c r="U986" s="1"/>
-      <c r="V986" s="1"/>
-      <c r="W986" s="1"/>
-      <c r="X986" s="1"/>
-      <c r="Y986" s="1"/>
-      <c r="Z986" s="1"/>
-    </row>
-    <row r="987" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A987" s="1"/>
-      <c r="B987" s="1"/>
-      <c r="C987" s="1"/>
-      <c r="D987" s="2"/>
-      <c r="E987" s="1"/>
-      <c r="F987" s="3"/>
-      <c r="G987" s="3"/>
-      <c r="H987" s="3"/>
-      <c r="I987" s="2"/>
-      <c r="J987" s="3"/>
-      <c r="K987" s="2"/>
-      <c r="L987" s="3"/>
-      <c r="M987" s="3"/>
-      <c r="N987" s="1"/>
-      <c r="O987" s="1"/>
-      <c r="P987" s="1"/>
-      <c r="Q987" s="1"/>
-      <c r="R987" s="1"/>
-      <c r="S987" s="1"/>
-      <c r="T987" s="1"/>
-      <c r="U987" s="1"/>
-      <c r="V987" s="1"/>
-      <c r="W987" s="1"/>
-      <c r="X987" s="1"/>
-      <c r="Y987" s="1"/>
-      <c r="Z987" s="1"/>
-    </row>
-    <row r="988" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A988" s="1"/>
-      <c r="B988" s="1"/>
-      <c r="C988" s="1"/>
-      <c r="D988" s="2"/>
-      <c r="E988" s="1"/>
-      <c r="F988" s="3"/>
-      <c r="G988" s="3"/>
-      <c r="H988" s="3"/>
-      <c r="I988" s="2"/>
-      <c r="J988" s="3"/>
-      <c r="K988" s="2"/>
-      <c r="L988" s="3"/>
-      <c r="M988" s="3"/>
-      <c r="N988" s="1"/>
-      <c r="O988" s="1"/>
-      <c r="P988" s="1"/>
-      <c r="Q988" s="1"/>
-      <c r="R988" s="1"/>
-      <c r="S988" s="1"/>
-      <c r="T988" s="1"/>
-      <c r="U988" s="1"/>
-      <c r="V988" s="1"/>
-      <c r="W988" s="1"/>
-      <c r="X988" s="1"/>
-      <c r="Y988" s="1"/>
-      <c r="Z988" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C45:C988 C21:C33 C17:C19 C1:C14" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C40:C983 C16:C28 C12:C14 C1:C9" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E21:E988 E17:E19 E1:E14" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E16:E983 E12:E14 E1:E9" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F21:F988 F17:F19 F1:F14" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F16:F983 F12:F14 F1:F9" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H21:H988 H17:H19 H1:H14" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H16:H983 H12:H14 H1:H9" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28471,7 +28216,7 @@
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="18"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>

</xml_diff>